<commit_message>
Update spreadsheet, adding stage details.
</commit_message>
<xml_diff>
--- a/2018_cpu/docs/AVR_rev1.xlsx
+++ b/2018_cpu/docs/AVR_rev1.xlsx
@@ -19,17 +19,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="152">
-  <si>
-    <t>ddddd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="165">
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ddddd</t>
+    <t>PASSB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1dddd</t>
+    <t>RF1MUX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC (ADD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC (ADC)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC (EOR)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASSB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -207,18 +267,12 @@
     <t>11dd</t>
   </si>
   <si>
-    <t>pseudo op (ADD)</t>
-  </si>
-  <si>
     <t>ROL</t>
   </si>
   <si>
     <t>Rd = Rd + Rd + C</t>
   </si>
   <si>
-    <t>pseudo op (ADC)</t>
-  </si>
-  <si>
     <t>SBC</t>
   </si>
   <si>
@@ -273,9 +327,6 @@
     <t>01dd</t>
   </si>
   <si>
-    <t>pseudo op (EOR)</t>
-  </si>
-  <si>
     <t>XOR</t>
   </si>
   <si>
@@ -430,9 +481,6 @@
   </si>
   <si>
     <t>AAAA</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>A</t>
@@ -474,10 +522,6 @@
   </si>
   <si>
     <t>DESC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>K</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -491,7 +535,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RFAMUX</t>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -513,12 +569,18 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -600,7 +662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -609,9 +671,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -621,6 +680,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1803,10 +1867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:IW58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13" customHeight="1"/>
@@ -1816,979 +1883,979 @@
     <col min="3" max="4" width="3.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
     <col min="6" max="9" width="5.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="1" customWidth="1"/>
     <col min="12" max="18" width="1.85546875" style="1" customWidth="1"/>
     <col min="19" max="19" width="2.140625" style="1" customWidth="1"/>
-    <col min="20" max="23" width="7.5703125" style="1" customWidth="1"/>
-    <col min="24" max="257" width="10.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="1" customWidth="1"/>
+    <col min="22" max="23" width="4.85546875" style="1" customWidth="1"/>
+    <col min="24" max="257" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>145</v>
+      <c r="A1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="6" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="2"/>
+        <v>158</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" customHeight="1">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1">
-      <c r="A2" s="16">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>21</v>
+      <c r="B2" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="4">
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15" customHeight="1">
-      <c r="A3" s="16">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>33</v>
+      <c r="A3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="4">
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1">
-      <c r="A4" s="16">
-        <v>1</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>36</v>
+      <c r="A4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15" customHeight="1">
-      <c r="A5" s="16">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>40</v>
+      <c r="A5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1">
-      <c r="A6" s="16">
-        <v>1</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>43</v>
+      <c r="A6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="4">
         <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1">
-      <c r="A7" s="16">
-        <v>1</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>48</v>
+      <c r="A7" s="13"/>
+      <c r="B7" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="4">
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W7" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15" customHeight="1">
-      <c r="A8" s="16">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>54</v>
+      <c r="A8" s="13"/>
+      <c r="B8" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="4">
         <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15" customHeight="1">
-      <c r="A9" s="16">
-        <v>1</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>56</v>
+      <c r="A9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="K9" s="4">
         <v>1</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15" customHeight="1">
-      <c r="A10" s="16">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>60</v>
+      <c r="A10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="K10" s="4">
         <v>1</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1">
-      <c r="A11" s="16">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>63</v>
+      <c r="A11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="4">
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15" customHeight="1">
-      <c r="A12" s="16">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>66</v>
+      <c r="A12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>5</v>
+        <v>80</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="4">
         <v>1</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" customHeight="1">
+      <c r="A13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1">
-      <c r="A13" s="16">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="4">
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15" customHeight="1">
-      <c r="A14" s="16">
-        <v>1</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>69</v>
+      <c r="A14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>7</v>
+        <v>83</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="4">
         <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15" customHeight="1">
-      <c r="A15" s="16"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -2812,8 +2879,8 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="15" customHeight="1">
-      <c r="A16" s="16"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2837,185 +2904,185 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" ht="15" customHeight="1">
-      <c r="A17" s="16">
-        <v>1</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>71</v>
+      <c r="A17" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="4">
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P17" s="4">
         <v>0</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="15" customHeight="1">
-      <c r="A18" s="16">
-        <v>1</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>75</v>
+      <c r="A18" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="4">
         <v>1</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P18" s="4">
         <v>0</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="15" customHeight="1">
-      <c r="A19" s="16">
-        <v>1</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>78</v>
+      <c r="A19" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>81</v>
+        <v>41</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="K19" s="4">
         <v>1</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O19" s="4">
         <v>0</v>
@@ -3030,231 +3097,231 @@
         <v>1</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="V19" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1">
-      <c r="A20" s="16">
-        <v>1</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>83</v>
+      <c r="A20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="4">
         <v>1</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P20" s="4">
         <v>0</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="V20" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1">
-      <c r="A21" s="16">
-        <v>1</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>85</v>
+      <c r="A21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="4">
         <v>1</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P21" s="4">
         <v>0</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V21" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="15" customHeight="1">
-      <c r="A22" s="16">
-        <v>1</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>87</v>
+      <c r="A22" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="4">
         <v>1</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P22" s="4">
         <v>0</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="U22" s="7" t="s">
-        <v>1</v>
+        <v>162</v>
       </c>
       <c r="V22" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="15" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -3278,8 +3345,8 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -3303,209 +3370,203 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1">
-      <c r="A25" s="16">
-        <v>1</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>90</v>
+      <c r="A25" s="13"/>
+      <c r="B25" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="4">
         <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1">
-      <c r="A26" s="16">
-        <v>1</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>92</v>
+      <c r="A26" s="13"/>
+      <c r="B26" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="4">
         <v>1</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q26" s="4">
         <v>0</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="U26" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V26" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="15" customHeight="1">
-      <c r="A27" s="16">
-        <v>1</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>93</v>
+      <c r="A27" s="13"/>
+      <c r="B27" s="19" t="s">
+        <v>105</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="3" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="4">
         <v>1</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R27" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="U27" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="15" customHeight="1">
-      <c r="A28" s="16"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -3529,8 +3590,8 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" ht="15" customHeight="1">
-      <c r="A29" s="16"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -3554,149 +3615,155 @@
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" ht="15" customHeight="1">
-      <c r="A30" s="16"/>
-      <c r="B30" s="12" t="s">
-        <v>94</v>
+      <c r="A30" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="D30" s="5">
         <v>41670</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="3" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="4">
         <v>0</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="U30" s="3"/>
       <c r="V30" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="15" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="12" t="s">
-        <v>100</v>
+      <c r="A31" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="D31" s="5">
         <v>41670</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="3" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="4">
         <v>0</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="U31" s="3"/>
       <c r="V31" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="28.5" customHeight="1">
-      <c r="A32" s="16"/>
-      <c r="B32" s="14" t="s">
-        <v>149</v>
+      <c r="A32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>159</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -3713,23 +3780,25 @@
       <c r="W32" s="2"/>
     </row>
     <row r="33" spans="1:23" ht="27.25" customHeight="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="14" t="s">
-        <v>150</v>
+      <c r="A33" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -3746,23 +3815,25 @@
       <c r="W33" s="2"/>
     </row>
     <row r="34" spans="1:23" ht="15" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="12" t="s">
-        <v>105</v>
+      <c r="A34" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -3779,23 +3850,25 @@
       <c r="W34" s="2"/>
     </row>
     <row r="35" spans="1:23" ht="15" customHeight="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="12" t="s">
-        <v>107</v>
+      <c r="A35" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="3" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -3812,23 +3885,25 @@
       <c r="W35" s="2"/>
     </row>
     <row r="36" spans="1:23" ht="15" customHeight="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="12" t="s">
-        <v>109</v>
+      <c r="A36" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="3" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -3845,23 +3920,25 @@
       <c r="W36" s="2"/>
     </row>
     <row r="37" spans="1:23" ht="15" customHeight="1">
-      <c r="A37" s="16"/>
-      <c r="B37" s="12" t="s">
-        <v>111</v>
+      <c r="A37" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="3" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -3878,23 +3955,25 @@
       <c r="W37" s="2"/>
     </row>
     <row r="38" spans="1:23" ht="15" customHeight="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="12" t="s">
-        <v>112</v>
+      <c r="A38" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="3" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -3911,23 +3990,25 @@
       <c r="W38" s="2"/>
     </row>
     <row r="39" spans="1:23" ht="15" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="12" t="s">
-        <v>114</v>
+      <c r="A39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="3" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -3944,23 +4025,25 @@
       <c r="W39" s="2"/>
     </row>
     <row r="40" spans="1:23" ht="15" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="12" t="s">
-        <v>115</v>
+      <c r="A40" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="3" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -3977,23 +4060,25 @@
       <c r="W40" s="2"/>
     </row>
     <row r="41" spans="1:23" ht="15" customHeight="1">
-      <c r="A41" s="16"/>
-      <c r="B41" s="12" t="s">
-        <v>116</v>
+      <c r="A41" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="3" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -4010,23 +4095,25 @@
       <c r="W41" s="2"/>
     </row>
     <row r="42" spans="1:23" ht="15" customHeight="1">
-      <c r="A42" s="16"/>
-      <c r="B42" s="12" t="s">
-        <v>118</v>
+      <c r="A42" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -4043,23 +4130,25 @@
       <c r="W42" s="2"/>
     </row>
     <row r="43" spans="1:23" ht="15" customHeight="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="12" t="s">
-        <v>119</v>
+      <c r="A43" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="3" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -4076,23 +4165,25 @@
       <c r="W43" s="2"/>
     </row>
     <row r="44" spans="1:23" ht="15" customHeight="1">
-      <c r="A44" s="16"/>
-      <c r="B44" s="12" t="s">
-        <v>120</v>
+      <c r="A44" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -4109,23 +4200,25 @@
       <c r="W44" s="2"/>
     </row>
     <row r="45" spans="1:23" ht="15" customHeight="1">
-      <c r="A45" s="16"/>
-      <c r="B45" s="12" t="s">
-        <v>122</v>
+      <c r="A45" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="3" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -4142,23 +4235,25 @@
       <c r="W45" s="2"/>
     </row>
     <row r="46" spans="1:23" ht="15" customHeight="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="12" t="s">
-        <v>123</v>
+      <c r="A46" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="3" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -4175,23 +4270,25 @@
       <c r="W46" s="2"/>
     </row>
     <row r="47" spans="1:23" ht="15" customHeight="1">
-      <c r="A47" s="16"/>
-      <c r="B47" s="12" t="s">
-        <v>125</v>
+      <c r="A47" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="3" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -4208,8 +4305,8 @@
       <c r="W47" s="2"/>
     </row>
     <row r="48" spans="1:23" ht="15" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="13"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -4233,8 +4330,8 @@
       <c r="W48" s="2"/>
     </row>
     <row r="49" spans="1:23" ht="15" customHeight="1">
-      <c r="A49" s="16"/>
-      <c r="B49" s="13"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -4258,69 +4355,71 @@
       <c r="W49" s="2"/>
     </row>
     <row r="50" spans="1:23" ht="15" customHeight="1">
-      <c r="A50" s="16"/>
-      <c r="B50" s="12" t="s">
-        <v>126</v>
+      <c r="A50" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="4">
         <v>2</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="4">
         <v>0</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="T50" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="U50" s="3"/>
       <c r="V50" s="3" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="W50" s="2"/>
     </row>
     <row r="51" spans="1:23" ht="15" customHeight="1">
-      <c r="A51" s="16"/>
-      <c r="B51" s="13"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -4344,8 +4443,8 @@
       <c r="W51" s="2"/>
     </row>
     <row r="52" spans="1:23" ht="15" customHeight="1">
-      <c r="A52" s="16"/>
-      <c r="B52" s="13"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -4369,262 +4468,272 @@
       <c r="W52" s="2"/>
     </row>
     <row r="53" spans="1:23" ht="15" customHeight="1">
-      <c r="A53" s="16"/>
-      <c r="B53" s="12" t="s">
-        <v>129</v>
+      <c r="A53" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="4">
         <v>1</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="4">
         <v>1</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T53" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="T53" s="3"/>
       <c r="U53" s="7" t="s">
-        <v>1</v>
+        <v>161</v>
       </c>
       <c r="V53" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="W53" s="2"/>
     </row>
     <row r="54" spans="1:23" ht="15" customHeight="1">
-      <c r="A54" s="16"/>
-      <c r="B54" s="12" t="s">
-        <v>136</v>
+      <c r="A54" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="4">
         <v>1</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T54" s="3" t="s">
-        <v>134</v>
+        <v>43</v>
+      </c>
+      <c r="T54" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="U54" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V54" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="W54" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="W54" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" spans="1:23" ht="15" customHeight="1">
-      <c r="A55" s="16"/>
-      <c r="B55" s="12" t="s">
-        <v>139</v>
+      <c r="A55" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="4">
         <v>1</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T55" s="3" t="s">
-        <v>134</v>
+        <v>43</v>
+      </c>
+      <c r="T55" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="U55" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
+        <v>161</v>
+      </c>
+      <c r="V55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="W55" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="1:23" ht="15" customHeight="1">
-      <c r="A56" s="16"/>
-      <c r="B56" s="12" t="s">
-        <v>141</v>
+      <c r="A56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="4">
         <v>1</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="J56" s="2"/>
       <c r="K56" s="4">
         <v>0</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T56" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="T56" s="3"/>
       <c r="U56" s="7" t="s">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="V56" s="3" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="W56" s="2"/>
     </row>
     <row r="57" spans="1:23" ht="15" customHeight="1">
-      <c r="A57" s="16"/>
-      <c r="B57" s="13"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="10"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -4648,9 +4757,11 @@
       <c r="W57" s="2"/>
     </row>
     <row r="58" spans="1:23" ht="15" customHeight="1">
-      <c r="A58" s="16"/>
-      <c r="B58" s="12" t="s">
-        <v>144</v>
+      <c r="A58" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="4">
@@ -4658,65 +4769,70 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="4">
         <v>0</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R58" s="3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T58" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="U58" s="3"/>
-      <c r="V58" s="2"/>
-      <c r="W58" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="T58" s="3"/>
+      <c r="U58" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="W58" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup scale="52" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>